<commit_message>
xlsx tables and config
</commit_message>
<xml_diff>
--- a/tables/xlsx/GameConfig.xlsx
+++ b/tables/xlsx/GameConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\Projects\Planetarium\NineChronicles\tables\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E67B434-D1FA-4FA3-A668-03006F58A297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60988F-8C64-4402-9AEF-B4A0FB1401CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,16 +60,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -77,22 +97,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -103,17 +174,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{922856E3-9B71-4211-9EB7-E5A013F95682}" name="GameConfigSheet" displayName="GameConfigSheet" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{922856E3-9B71-4211-9EB7-E5A013F95682}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DD2096D5-9681-41EE-8BFC-7C2BB1D187D8}" name="key" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{5C7FB3A0-244C-4E8D-8191-A5CCF913CDD7}" name="value"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,9 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F86554-558F-4D09-AF17-8AB4171D15A5}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -392,58 +450,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1700</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>56000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>